<commit_message>
Add TypeScript interfaces, update app structure, and enhance theme support
</commit_message>
<xml_diff>
--- a/server/input/New_Spreadsheet_1.xlsx
+++ b/server/input/New_Spreadsheet_1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>General Journal</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Account No.</t>
+  </si>
+  <si>
+    <t>ITEMS</t>
   </si>
   <si>
     <t>BALANCE</t>
@@ -462,9 +465,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.5703125" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" customWidth="1"/>
-    <col min="4" max="6" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -514,9 +520,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="9" width="7.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -537,7 +547,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>3</v>
@@ -549,7 +559,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -579,13 +589,13 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -595,7 +605,7 @@
     <row r="5" spans="1:2">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -605,7 +615,7 @@
     <row r="8" spans="1:2">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -615,7 +625,7 @@
     <row r="11" spans="1:2">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -625,7 +635,7 @@
     <row r="14" spans="1:2">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:2">

</xml_diff>